<commit_message>
finished total deduction and ot computations
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
@@ -9,12 +9,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="52">
   <si>
     <t>iRipple, Inc.</t>
   </si>
   <si>
-    <t>Name: Arceo,Arwin</t>
+    <t>Name: Arceo, Arwin</t>
   </si>
   <si>
     <t>Department: Project - International</t>
@@ -50,62 +50,79 @@
     <t>REMARKS</t>
   </si>
   <si>
-    <t>02-10-2015</t>
+    <t>03-21-2015</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t> Others|Mydin live integration for all Branches.|
+</t>
+  </si>
+  <si>
+    <t>03-22-2015</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>03-23-2015</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>03-24-2015</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t> Others|Mydin SAP Integration Live.|
+    <t>03-25-2015</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>03-26-2015</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>03-27-2015</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>03-28-2015</t>
+  </si>
+  <si>
+    <t>03-29-2015</t>
+  </si>
+  <si>
+    <t>03-30-2015</t>
+  </si>
+  <si>
+    <t>03-31-2015</t>
+  </si>
+  <si>
+    <t>04-01-2015</t>
+  </si>
+  <si>
+    <t> Rest and vacation with my family.
 </t>
   </si>
   <si>
-    <t>02-11-2015</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>02-12-2015</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>02-13-2015</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>02-14-2015</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>02-15-2015</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>02-16-2015</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>02-17-2015</t>
-  </si>
-  <si>
-    <t>02-18-2015</t>
-  </si>
-  <si>
-    <t>02-19-2015</t>
-  </si>
-  <si>
-    <t>02-20-2015</t>
+    <t>04-02-2015</t>
+  </si>
+  <si>
+    <t>
+</t>
+  </si>
+  <si>
+    <t>04-03-2015</t>
   </si>
   <si>
     <t>NUMBER OF TIMES TARDY</t>
@@ -121,6 +138,9 @@
   </si>
   <si>
     <t>TOTAL LEAVES ACCUMULATED</t>
+  </si>
+  <si>
+    <t>@@cut_off_date.to_date.mon &gt;= self.date_start.to_date.mon &amp;&amp; @@cut_off_date.to_date.mon &lt;= self.date_end.to_date.mon</t>
   </si>
   <si>
     <t>ACCUMULATED OT</t>
@@ -264,14 +284,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="46.82022471910113"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="86.68988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.884831460674157"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.184831460674157"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="24.434831460674157"/>
@@ -279,7 +299,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="34.33483146067415"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="24.434831460674157"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="17.834831460674156"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="30.58988764044944"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="34.98988764044944"/>
     <col min="11" max="11" bestFit="false" customWidth="false" hidden="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="4.189887640449439" hidden="true"/>
     <col min="13" max="13" bestFit="false" customWidth="false" hidden="true"/>
@@ -344,9 +364,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -370,9 +388,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -396,9 +412,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -422,9 +436,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -448,9 +460,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F9" s="5"/>
       <c r="G9" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -474,9 +484,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F10" s="5"/>
       <c r="G10" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -500,9 +508,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F11" s="5"/>
       <c r="G11" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -526,9 +532,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -552,9 +556,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F13" s="5"/>
       <c r="G13" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -578,9 +580,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F14" s="5"/>
       <c r="G14" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -604,9 +604,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5" t="n">
         <v>0.0</v>
       </c>
@@ -625,28 +623,20 @@
         <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="5" t="str">
-        <f>COUNT(F5:F15)</f>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>0.0</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>33</v>
@@ -657,269 +647,208 @@
         <v>34</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="5" t="str">
-        <f>SUM(F5:F15)</f>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="5" t="n">
+        <v>0.0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I18" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="5" t="str">
-        <f>SUM(G5:G15)</f>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="F19" s="5" t="str">
+        <f>COUNT(F5:F18)</f>
       </c>
       <c r="G19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="5" t="str">
-        <f>SUM(H5:H15)</f>
-      </c>
-      <c r="I19" s="5" t="str">
-        <f>SUM(I5:I15)</f>
+        <v>38</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="5" t="str">
+        <f>SUM(F5:F18)</f>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <f>FLOOR(G18/8,1,1)&amp;"."&amp;FLOOR(MOD(G18,8),1,1)&amp;"."&amp;(MOD(G18,8)-FLOOR(MOD(G18,8),1,1))*60</f>
+        <v>40</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="G21" s="5" t="str">
+        <f>SUM(G5:G18)</f>
       </c>
       <c r="H21" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K21" s="5" t="str">
-        <f>INT(LEFT(B22,1))</f>
-      </c>
-      <c r="L21" s="5" t="str">
-        <f>RIGHT(B22,LEN(B22)-2)</f>
-      </c>
-      <c r="M21" s="5" t="str">
-        <f>INT(LEFT(L21,1))</f>
-      </c>
-      <c r="N21" s="5" t="str">
-        <f>RIGHT(L21,LEN(L21)-2)+0</f>
-      </c>
-      <c r="O21" s="5" t="str">
-        <f>K21*8*60+M21*60+N21</f>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="5" t="str">
-        <f>FLOOR(F17/8,1,1)&amp;"."&amp;FLOOR(MOD(F17,8),1,1)&amp;"."&amp;(MOD(F17,8)-FLOOR(MOD(F17,8),1,1))*60</f>
+        <v>41</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="H22" s="5" t="str">
+        <f>SUM(H5:H14)</f>
+      </c>
+      <c r="I22" s="5" t="str">
+        <f>SUM(I5:I14)</f>
       </c>
       <c r="J22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="5" t="str">
-        <f>INT(LEFT(B23,1))</f>
-      </c>
-      <c r="L22" s="5" t="str">
-        <f>RIGHT(B23,LEN(B23)-2)</f>
-      </c>
-      <c r="M22" s="5" t="str">
-        <f>INT(LEFT(L22,1))</f>
-      </c>
-      <c r="N22" s="5" t="str">
-        <f>RIGHT(L22,LEN(L22)-2)+0</f>
-      </c>
-      <c r="O22" s="5" t="str">
-        <f>K22*8*60+M22*60+N22</f>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <f>FLOOR(H19,1,1)&amp;"."&amp;(H19-FLOOR(H19,1,1))*8&amp;".0"</f>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K23" s="5" t="str">
-        <f>INT(LEFT(B24,1))</f>
-      </c>
-      <c r="L23" s="5" t="str">
-        <f>RIGHT(B24,LEN(B24)-2)</f>
-      </c>
-      <c r="M23" s="5" t="str">
-        <f>INT(LEFT(L23,1))</f>
-      </c>
-      <c r="N23" s="5" t="str">
-        <f>RIGHT(L23,LEN(L23)-2)+0</f>
-      </c>
-      <c r="O23" s="5" t="str">
-        <f>K23*8*60+M23*60+N23</f>
-      </c>
-    </row>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23"/>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24" s="5" t="str">
-        <f>FLOOR(I19,1,1)&amp;"."&amp;(I19-FLOOR(I19,1,1))*8&amp;".0"</f>
+        <f>FLOOR(G21/8,1,1)&amp;"."&amp;FLOOR(MOD(G21,8),1,1)&amp;"."&amp;(MOD(G21,8)-FLOOR(MOD(G21,8),1,1))*60</f>
       </c>
       <c r="C24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="K24" s="5" t="str">
         <f>INT(LEFT(B25,1))</f>
@@ -939,34 +868,34 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f>FLOOR(F20/8,1,1)&amp;"."&amp;FLOOR(MOD(F20,8),1,1)&amp;"."&amp;(MOD(F20,8)-FLOOR(MOD(F20,8),1,1))*60</f>
       </c>
       <c r="C25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="K25" s="5" t="str">
         <f>INT(LEFT(B26,1))</f>
@@ -986,84 +915,225 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f>FLOOR(H22,1,1)&amp;"."&amp;(H22-FLOOR(H22,1,1))*8&amp;".0"</f>
       </c>
       <c r="C26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="K26" s="5" t="str">
-        <f>K21+IF(K22&gt;K24,K22-K24,0)+IF(K23&gt;K25,K23-K25,0)</f>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>33</v>
+        <f>INT(LEFT(B27,1))</f>
+      </c>
+      <c r="L26" s="5" t="str">
+        <f>RIGHT(B27,LEN(B27)-2)</f>
       </c>
       <c r="M26" s="5" t="str">
-        <f>M21+IF(M22&gt;M24,M22-M24,0)+IF(M23&gt;M25,M23-M25,0)</f>
+        <f>INT(LEFT(L26,1))</f>
       </c>
       <c r="N26" s="5" t="str">
-        <f>N21+IF(N22&gt;N24,N22-N24,0)+IF(N23&gt;N25,N23-N25,0)</f>
+        <f>RIGHT(L26,LEN(L26)-2)+0</f>
       </c>
       <c r="O26" s="5" t="str">
-        <f>O21+IF(O22&gt;O24,O22-O24,0)+IF(O23&gt;O25,O23-O25,0)</f>
+        <f>K26*8*60+M26*60+N26</f>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="5" t="str">
-        <f>FLOOR(K27/8,1,1)&amp;"."&amp;FLOOR(MOD(K27,8),1,1)&amp;"."&amp;(MOD(K27,8)-FLOOR(MOD(K27,8),1,1))*60</f>
+        <f>FLOOR(I22,1,1)&amp;"."&amp;(I22-FLOOR(I22,1,1))*8&amp;".0"</f>
       </c>
       <c r="C27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="K27" s="5" t="str">
-        <f>O26/60</f>
+        <f>INT(LEFT(B28,1))</f>
+      </c>
+      <c r="L27" s="5" t="str">
+        <f>RIGHT(B28,LEN(B28)-2)</f>
+      </c>
+      <c r="M27" s="5" t="str">
+        <f>INT(LEFT(L27,1))</f>
+      </c>
+      <c r="N27" s="5" t="str">
+        <f>RIGHT(L27,LEN(L27)-2)+0</f>
+      </c>
+      <c r="O27" s="5" t="str">
+        <f>K27*8*60+M27*60+N27</f>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K28" s="5" t="str">
+        <f>INT(LEFT(B29,1))</f>
+      </c>
+      <c r="L28" s="5" t="str">
+        <f>RIGHT(B29,LEN(B29)-2)</f>
+      </c>
+      <c r="M28" s="5" t="str">
+        <f>INT(LEFT(L28,1))</f>
+      </c>
+      <c r="N28" s="5" t="str">
+        <f>RIGHT(L28,LEN(L28)-2)+0</f>
+      </c>
+      <c r="O28" s="5" t="str">
+        <f>K28*8*60+M28*60+N28</f>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" s="5" t="str">
+        <f>K24+IF(K25&gt;K27,K25-K27,0)+IF(K26&gt;K28,K26-K28,0)</f>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M29" s="5" t="str">
+        <f>M24+IF(M25&gt;M27,M25-M27,0)+IF(M26&gt;M28,M26-M28,0)</f>
+      </c>
+      <c r="N29" s="5" t="str">
+        <f>N24+IF(N25&gt;N27,N25-N27,0)+IF(N26&gt;N28,N26-N28,0)</f>
+      </c>
+      <c r="O29" s="5" t="str">
+        <f>O24+IF(O25&gt;O27,O25-O27,0)+IF(O26&gt;O28,O26-O28,0)</f>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="5" t="str">
+        <f>FLOOR(K30/8,1,1)&amp;"."&amp;FLOOR(MOD(K30,8),1,1)&amp;"."&amp;(MOD(K30,8)-FLOOR(MOD(K30,8),1,1))*60</f>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K30" s="5" t="str">
+        <f>O29/60</f>
       </c>
     </row>
   </sheetData>
@@ -1072,13 +1142,13 @@
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>

</xml_diff>

<commit_message>
Attempted adding loading screen in download
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="60">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Saturday</t>
-  </si>
-  <si>
-    <t>01:00:00</t>
   </si>
   <si>
     <t>08:30:00</t>
@@ -520,33 +517,29 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N5" s="6"/>
       <c r="O5" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -556,33 +549,29 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="6"/>
+      <c r="L6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="M6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="N6" s="6"/>
       <c r="O6" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -592,33 +581,29 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="6"/>
+      <c r="L7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N7" s="6"/>
       <c r="O7" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -628,33 +613,29 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="6"/>
+      <c r="L8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="M8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N8" s="6"/>
       <c r="O8" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -664,33 +645,29 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N9" s="6"/>
       <c r="O9" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -700,33 +677,29 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="6"/>
+      <c r="L10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="M10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N10" s="6"/>
       <c r="O10" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -736,30 +709,26 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="6" t="s">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="M11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="N11" s="6"/>
       <c r="O11" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>20</v>
@@ -772,33 +741,29 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="6"/>
+      <c r="L12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="M12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N12" s="6"/>
       <c r="O12" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -808,33 +773,29 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="6"/>
+      <c r="L13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="M13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="N13" s="6"/>
       <c r="O13" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -844,33 +805,29 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="6"/>
+      <c r="L14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="M14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N14" s="6"/>
       <c r="O14" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -880,33 +837,29 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="6" t="s">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="N15" s="6"/>
       <c r="O15" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -928,15 +881,15 @@
         </is>
       </c>
       <c r="P16" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -965,10 +918,10 @@
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -997,175 +950,175 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="5" t="str">
         <f>COUNT(E5:E15)</f>
       </c>
       <c r="F19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="5" t="str">
         <f>SUM(E5:E15)</f>
       </c>
       <c r="F20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G21" s="5" t="str">
         <f>SUM(G5:G18)</f>
       </c>
       <c r="H21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H22" s="5" t="str">
         <f>SUM(H5:H15)</f>
@@ -1174,76 +1127,76 @@
         <f>SUM(I5:I15)</f>
       </c>
       <c r="J22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23"/>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5" t="str">
         <f>FLOOR(G21/8,1)&amp;"."&amp;FLOOR(MOD(G21,8),1)&amp;"."&amp;(MOD(G21,8)-FLOOR(MOD(G21,8),1))*60</f>
       </c>
       <c r="D24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q24" s="0" t="str">
         <f>INT(LEFT(C25,2))</f>
@@ -1263,52 +1216,52 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="5" t="str">
         <f>FLOOR(E20/8,1)&amp;"."&amp;FLOOR(MOD(E20,8),1)&amp;"."&amp;(MOD(E20,8)-FLOOR(MOD(E20,8),1))*60</f>
       </c>
       <c r="D25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q25" s="0" t="str">
         <f>INT(LEFT(C26,2))</f>
@@ -1328,52 +1281,52 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5" t="str">
         <f>FLOOR(H22,1)&amp;"."&amp;(H22-FLOOR(H22,1))*8&amp;".0"</f>
       </c>
       <c r="D26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q26" s="0" t="str">
         <f>INT(LEFT(C27,2))</f>
@@ -1393,52 +1346,52 @@
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="5" t="str">
         <f>FLOOR(I22,1)&amp;"."&amp;(I22-FLOOR(I22,1))*8&amp;".0"</f>
       </c>
       <c r="D27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q27" s="0" t="str">
         <f>INT(LEFT(C28,2))</f>
@@ -1458,52 +1411,52 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q28" s="0" t="str">
         <f>INT(LEFT(C29,2))</f>
@@ -1523,58 +1476,58 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="D29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q29" s="0" t="str">
         <f>Q24+IF(Q25&gt;Q27,Q25-Q27,0)+IF(Q26&gt;Q28,Q26-Q28,0)</f>
       </c>
       <c r="R29" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S29" s="0" t="str">
         <f>S24+IF(S25&gt;S27,S25-S27,0)+IF(S26&gt;S28,S26-S28,0)</f>
@@ -1588,52 +1541,52 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="5" t="str">
         <f>FLOOR(Q30/8,1)&amp;"."&amp;FLOOR(MOD(Q30,8),1)&amp;"."&amp;(MOD(Q30,8)-FLOOR(MOD(Q30,8),1))*60</f>
       </c>
       <c r="D30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q30" s="0" t="str">
         <f>U29/60</f>

</xml_diff>

<commit_message>
Fixed late error, commented out delete all button
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="57" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="66" xml:space="preserve">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -89,13 +89,22 @@
     <t>Monday</t>
   </si>
   <si>
+    <t>07:18:53</t>
+  </si>
+  <si>
+    <t>19:25:46</t>
+  </si>
+  <si>
     <t>04-28-2015</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>12:09:00</t>
+    <t>07:08:19</t>
+  </si>
+  <si>
+    <t>18:42:35</t>
   </si>
   <si>
     <t>04-29-2015</t>
@@ -104,12 +113,24 @@
     <t>Wednesday</t>
   </si>
   <si>
+    <t>07:24:56</t>
+  </si>
+  <si>
+    <t>18:59:59</t>
+  </si>
+  <si>
     <t>04-30-2015</t>
   </si>
   <si>
     <t>Thursday</t>
   </si>
   <si>
+    <t>07:07:59</t>
+  </si>
+  <si>
+    <t>17:23:13</t>
+  </si>
+  <si>
     <t>05-01-2015</t>
   </si>
   <si>
@@ -126,6 +147,12 @@
   </si>
   <si>
     <t>05-04-2015</t>
+  </si>
+  <si>
+    <t>07:04:16</t>
+  </si>
+  <si>
+    <t>11:15:23</t>
   </si>
   <si>
     <t>05-05-2015</t>
@@ -556,130 +583,138 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P7" s="8" t="inlineStr">
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P7" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P8" s="7" t="inlineStr">
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P8" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P9" s="8" t="inlineStr">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P9" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P10" s="8" t="inlineStr">
+      <c r="A10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P10" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -687,10 +722,10 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -710,12 +745,12 @@
         </is>
       </c>
       <c r="P11" s="6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
@@ -745,7 +780,7 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>22</v>
@@ -774,32 +809,36 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P14" s="8" t="inlineStr">
+      <c r="C14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P14" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -807,10 +846,10 @@
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -839,10 +878,10 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -871,10 +910,10 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -903,10 +942,10 @@
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -935,175 +974,175 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E19" s="5" t="str">
         <f>COUNT(E5:E18)</f>
       </c>
       <c r="F19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E20" s="5" t="str">
         <f>SUM(E5:E18)</f>
       </c>
       <c r="F20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G21" s="5" t="str">
         <f>SUM(G5:G18)</f>
       </c>
       <c r="H21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H22" s="5" t="str">
         <f>SUM(H5:H18)</f>
@@ -1112,76 +1151,76 @@
         <f>SUM(I5:I18)</f>
       </c>
       <c r="J22" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23"/>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5" t="str">
         <f>FLOOR(G21/8,1)&amp;"."&amp;FLOOR(MOD(G21,8),1)&amp;"."&amp;(MOD(G21,8)-FLOOR(MOD(G21,8),1))*60</f>
       </c>
       <c r="D24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q24" s="0" t="str">
         <f>INT(LEFT(C25,2))</f>
@@ -1201,52 +1240,52 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C25" s="5" t="str">
         <f>FLOOR(E20/8,1)&amp;"."&amp;FLOOR(MOD(E20,8),1)&amp;"."&amp;(MOD(E20,8)-FLOOR(MOD(E20,8),1))*60</f>
       </c>
       <c r="D25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q25" s="0" t="str">
         <f>INT(LEFT(C26,2))</f>
@@ -1266,52 +1305,52 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5" t="str">
         <f>FLOOR(H22,1)&amp;"."&amp;(H22-FLOOR(H22,1))*8&amp;".0"</f>
       </c>
       <c r="D26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q26" s="0" t="str">
         <f>INT(LEFT(C27,2))</f>
@@ -1331,52 +1370,52 @@
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C27" s="5" t="str">
         <f>FLOOR(I22,1)&amp;"."&amp;(I22-FLOOR(I22,1))*8&amp;".0"</f>
       </c>
       <c r="D27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q27" s="0" t="str">
         <f>INT(LEFT(C28,2))</f>
@@ -1396,52 +1435,52 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q28" s="0" t="str">
         <f>INT(LEFT(C29,2))</f>
@@ -1461,58 +1500,58 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q29" s="0" t="str">
         <f>Q24+IF(Q25&gt;Q27,Q25-Q27,0)+IF(Q26&gt;Q28,Q26-Q28,0)</f>
       </c>
       <c r="R29" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="S29" s="0" t="str">
         <f>S24+IF(S25&gt;S27,S25-S27,0)+IF(S26&gt;S28,S26-S28,0)</f>
@@ -1526,52 +1565,52 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C30" s="5" t="str">
         <f>FLOOR(Q30/8,1)&amp;"."&amp;FLOOR(MOD(Q30,8),1)&amp;"."&amp;(MOD(Q30,8)-FLOOR(MOD(Q30,8),1))*60</f>
       </c>
       <c r="D30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q30" s="0" t="str">
         <f>U29/60</f>

</xml_diff>

<commit_message>
added absences in computation of total deduction
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Arceo,Arwin.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="70" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="71" xml:space="preserve">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>TOTAL LEAVES ACCUMULATED</t>
+  </si>
+  <si>
+    <t>TOTAL ABSENCES</t>
   </si>
   <si>
     <t>ACCUMULATED OT</t>
@@ -465,7 +468,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0">
       <pane topLeftCell="C5" state="frozenSplit" activePane="bottomRight" ySplit="4" xSplit="2"/>
@@ -1201,119 +1204,106 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23"/>
-    <row r="24">
-      <c r="A24" s="13" t="s">
+    <row r="23">
+      <c r="A23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="5" t="str">
-        <f>FLOOR(G21/8,1)&amp;"."&amp;FLOOR(MOD(G21,8),1)&amp;"."&amp;(MOD(G21,8)-FLOOR(MOD(G21,8),1))*60</f>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q24" s="0" t="str">
-        <f>INT(LEFT(C25,2))</f>
-      </c>
-      <c r="R24" s="0" t="str">
-        <f>IF(LEFT(RIGHT(C25,LEN(C25)-2),1)=".",RIGHT(C25,LEN(C25)-3),RIGHT(C25,LEN(C25)-2))</f>
-      </c>
-      <c r="S24" s="0" t="str">
-        <f>INT(LEFT(R24,1))</f>
-      </c>
-      <c r="T24" s="0" t="str">
-        <f>RIGHT(R24,LEN(R24)-2)+0</f>
-      </c>
-      <c r="U24" s="0" t="str">
-        <f>Q24*8*60+S24*60+T24</f>
-      </c>
-    </row>
+      <c r="B23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24"/>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="5" t="str">
-        <f>FLOOR(E20/8,1)&amp;"."&amp;FLOOR(MOD(E20,8),1)&amp;"."&amp;(MOD(E20,8)-FLOOR(MOD(E20,8),1))*60</f>
+        <f>FLOOR(G21/8,1)&amp;"."&amp;FLOOR(MOD(G21,8),1)&amp;"."&amp;(MOD(G21,8)-FLOOR(MOD(G21,8),1))*60</f>
       </c>
       <c r="D25" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="P25" s="12" t="s">
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P25" s="3" t="s">
         <v>53</v>
       </c>
       <c r="Q25" s="0" t="str">
@@ -1334,51 +1324,51 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="5" t="str">
-        <f>FLOOR(H22,1)&amp;"."&amp;(H22-FLOOR(H22,1))*8&amp;".0"</f>
+        <f>FLOOR(I23,1,1)&amp;"."&amp;FLOOR(MOD(I23*8,8),1,1)&amp;"."&amp;(MOD(I23*8,8)-FLOOR(MOD(I23*8,8),1,1))*60</f>
       </c>
       <c r="D26" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="M26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="P26" s="12" t="s">
+      <c r="E26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>53</v>
       </c>
       <c r="Q26" s="0" t="str">
@@ -1399,22 +1389,22 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="5" t="str">
-        <f>FLOOR(I22,1)&amp;"."&amp;(I22-FLOOR(I22,1))*8&amp;".0"</f>
+        <f>FLOOR(E20/8,1)&amp;"."&amp;FLOOR(MOD(E20,8),1)&amp;"."&amp;(MOD(E20,8)-FLOOR(MOD(E20,8),1))*60</f>
       </c>
       <c r="D27" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>53</v>
@@ -1464,18 +1454,18 @@
     </row>
     <row r="28">
       <c r="A28" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>65</v>
+      <c r="C28" s="5" t="str">
+        <f>FLOOR(H22,1)&amp;"."&amp;(H22-FLOOR(H22,1))*8&amp;".0"</f>
       </c>
       <c r="D28" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F28" s="12" t="s">
@@ -1529,22 +1519,22 @@
     </row>
     <row r="29">
       <c r="A29" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>67</v>
+      <c r="C29" s="5" t="str">
+        <f>FLOOR(I22,1)&amp;"."&amp;(I22-FLOOR(I22,1))*8&amp;".0"</f>
       </c>
       <c r="D29" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>53</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>53</v>
@@ -1577,77 +1567,207 @@
         <v>53</v>
       </c>
       <c r="Q29" s="0" t="str">
-        <f>Q24+IF(Q25&gt;Q27,Q25-Q27,0)+IF(Q26&gt;Q28,Q26-Q28,0)</f>
-      </c>
-      <c r="R29" s="0" t="s">
-        <v>53</v>
+        <f>INT(LEFT(C30,2))</f>
+      </c>
+      <c r="R29" s="0" t="str">
+        <f>IF(LEFT(RIGHT(C30,LEN(C30)-2),1)=".",RIGHT(C30,LEN(C30)-3),RIGHT(C30,LEN(C30)-2))</f>
       </c>
       <c r="S29" s="0" t="str">
-        <f>S24+IF(S25&gt;S27,S25-S27,0)+IF(S26&gt;S28,S26-S28,0)</f>
+        <f>INT(LEFT(R29,1))</f>
       </c>
       <c r="T29" s="0" t="str">
-        <f>T24+IF(T25&gt;T27,T25-T27,0)+IF(T26&gt;T28,T26-T28,0)</f>
+        <f>RIGHT(R29,LEN(R29)-2)+0</f>
       </c>
       <c r="U29" s="0" t="str">
-        <f>U24+IF(U25&gt;U27,U25-U27,0)+IF(U26&gt;U28,U26-U28,0)</f>
+        <f>Q29*8*60+S29*60+T29</f>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q30" s="0" t="str">
+        <f>INT(LEFT(C31,2))</f>
+      </c>
+      <c r="R30" s="0" t="str">
+        <f>IF(LEFT(RIGHT(C31,LEN(C31)-2),1)=".",RIGHT(C31,LEN(C31)-3),RIGHT(C31,LEN(C31)-2))</f>
+      </c>
+      <c r="S30" s="0" t="str">
+        <f>INT(LEFT(R30,1))</f>
+      </c>
+      <c r="T30" s="0" t="str">
+        <f>RIGHT(R30,LEN(R30)-2)+0</f>
+      </c>
+      <c r="U30" s="0" t="str">
+        <f>Q30*8*60+S30*60+T30</f>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="5" t="str">
-        <f>FLOOR(Q30/8,1)&amp;"."&amp;FLOOR(MOD(Q30,8),1)&amp;"."&amp;(MOD(Q30,8)-FLOOR(MOD(Q30,8),1))*60</f>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="P30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q30" s="0" t="str">
-        <f>U29/60</f>
+      <c r="G31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="P31" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q31" s="0" t="str">
+        <f>Q26+Q25+IF(Q27&gt;Q29,Q27-Q29,0)+IF(Q28&gt;Q30,Q28-Q30,0)</f>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="S31" s="0" t="str">
+        <f>S26+S25+IF(S27&gt;S29,S27-S29,0)+IF(S28&gt;S30,S28-S30,0)</f>
+      </c>
+      <c r="T31" s="0" t="str">
+        <f>T26+T25+IF(T27&gt;T29,T27-T29,0)+IF(T28&gt;T30,T28-T30,0)</f>
+      </c>
+      <c r="U31" s="0" t="str">
+        <f>U26+U25+IF(U27&gt;U29,U27-U29,0)+IF(U28&gt;U30,U28-U30,0)</f>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="5" t="str">
+        <f>FLOOR(Q32/8,1)&amp;"."&amp;FLOOR(MOD(Q32,8),1)&amp;"."&amp;(MOD(Q32,8)-FLOOR(MOD(Q32,8),1))*60</f>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q32" s="0" t="str">
+        <f>U31/60</f>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="25">
+  <mergeCells count="28">
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A3:P3"/>
@@ -1659,12 +1779,11 @@
     <mergeCell ref="H21:P21"/>
     <mergeCell ref="A22:G22"/>
     <mergeCell ref="J22:P22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="E24:P24"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="J23:P23"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:P26"/>
     <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E26:P26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="F27:P28"/>
@@ -1673,6 +1792,10 @@
     <mergeCell ref="E29:E30"/>
     <mergeCell ref="F29:P30"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:P32"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>

</xml_diff>